<commit_message>
add lead comb info
</commit_message>
<xml_diff>
--- a/pydata/comb_data_input.xlsx
+++ b/pydata/comb_data_input.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="98">
   <si>
     <t>价格分摊</t>
   </si>
@@ -54,18 +54,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>ZH20210219A66</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ZH20210219A66</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>白色PZ手提箱蕾丝包裙N白飞袖双蝴蝶裙+白镂空短爬 发带围嘴裤袜白袜菠萝毯59</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>parkzoo</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -78,7 +66,116 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>KC20190720A0201</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KC20190612A01</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KC20201217A01</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KC20200301A05</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KC20200729D01</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KC20210219A02</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KC20190521A0102</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KC20210509A0202</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KC20190521A0103</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KC20190720A0202</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KC20210509A0203</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KC20190521A0104</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KC20210509A0204</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KC20200425A0101</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KC20200425A0102</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KC20200425A0103</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KC20200425A0104</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KC20210408A0201</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KC20210219A01</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KC20210408A0202</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KC20210408A0203</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KC20210408A0204</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZHTM20210218A66</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZHTM20210218A66</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>天猫-白色PZ手提箱蕾丝包裙N白飞袖双蝴蝶裙+白镂空短爬 发带围嘴裤袜白袜菠萝毯59</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>parkzoo</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>白色PZ手提箱蕾丝裙</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>白色飞袖双蝴蝶结蕾丝连衣裙66</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>KC20190521A0101</t>
@@ -86,34 +183,23 @@
   </si>
   <si>
     <t>镂空花瓣带帽短袖哈衣8276#59</t>
-  </si>
-  <si>
-    <t>KC20190720A0201</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>白色开档针织连裤袜小号</t>
-  </si>
-  <si>
-    <t>KC20190612A01</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>白色菠萝格毛毯</t>
-  </si>
-  <si>
-    <t>KC20201217A01</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>白色PARKZOO手提箱</t>
-  </si>
-  <si>
-    <t>KC20200301A05</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>刺绣sweety360度围嘴</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>KC20200729D01</t>
@@ -121,6 +207,47 @@
   </si>
   <si>
     <t>立体金色皇冠网纱蝴蝶结发带42135#</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>白色蝴蝶结袜子</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZHTM20210218A67</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>天猫-白色PZ手提箱蕾丝包裙N白飞袖双蝴蝶裙+白镂空短爬 发带围嘴裤袜白袜菠萝毯66</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>镂空花瓣带帽短袖哈衣8276#66</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>白色PARKZOO手提箱</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZHTM20210218A68</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>天猫-白色PZ手提箱蕾丝包裙N白飞袖双蝴蝶裙+白镂空短爬 发带围嘴裤袜白袜菠萝毯73</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>白色飞袖双蝴蝶结蕾丝连衣裙73</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>镂空花瓣带帽短袖哈衣8276#73</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>白色开档针织连裤袜大号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>KC20210219A02</t>
@@ -128,269 +255,154 @@
   </si>
   <si>
     <t>白色蝴蝶结袜子</t>
-  </si>
-  <si>
-    <t>ZH20210219A67</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>白色PZ手提箱蕾丝包裙N白飞袖双蝴蝶裙+白镂空短爬 发带围嘴裤袜白袜菠萝毯66</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>parkzoo</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>白色PZ手提箱蕾丝裙</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>KC20190521A0102</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>镂空花瓣带帽短袖哈衣8276#66</t>
-  </si>
-  <si>
-    <t>KC20200301A05</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>KC20200729D01</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>KC20210219A02</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ZH20210219A68</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>白色PZ手提箱蕾丝包裙N白飞袖双蝴蝶裙+白镂空短爬 发带围嘴裤袜白袜菠萝毯73</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>parkzoo</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>白色PZ手提箱蕾丝裙</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>KC20210509A0202</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>白色飞袖双蝴蝶结蕾丝连衣裙73</t>
-  </si>
-  <si>
-    <t>KC20190521A0103</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>镂空花瓣带帽短袖哈衣8276#73</t>
-  </si>
-  <si>
-    <t>KC20190720A0202</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>白色开档针织连裤袜大号</t>
-  </si>
-  <si>
-    <t>ZH20210219A69</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>白色PZ手提箱蕾丝包裙N白飞袖双蝴蝶裙+白镂空短爬 发带围嘴裤袜白袜菠萝毯80</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>KC20210509A0203</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZHTM20210218A69</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>天猫-白色PZ手提箱蕾丝包裙N白飞袖双蝴蝶裙+白镂空短爬 发带围嘴裤袜白袜菠萝毯80</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>白色飞袖双蝴蝶结蕾丝连衣裙80</t>
-  </si>
-  <si>
-    <t>KC20190521A0104</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>镂空花瓣带帽短袖哈衣8276#80</t>
-  </si>
-  <si>
-    <t>ZH20210219A70</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>白色PZ手提箱蕾丝包裙N白飞袖双蝴蝶裙+白镂空短爬 发带围嘴裤袜白袜菠萝毯90</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>KC20210509A0204</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZHTM20210218A70</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>天猫-白色PZ手提箱蕾丝包裙N白飞袖双蝴蝶裙+白镂空短爬 发带围嘴裤袜白袜菠萝毯90</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>白色飞袖双蝴蝶结蕾丝连衣裙90</t>
-  </si>
-  <si>
-    <t>ZH20210219A71</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>白色PZ手提箱蕾丝包裙O白飞袖双蝴蝶裙+白无袖爬 发带围嘴裤袜白袜菠萝毯59</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>KC20200425A0101</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZHTM20210218A71</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>天猫-白色PZ手提箱蕾丝包裙O白飞袖双蝴蝶裙+白无袖爬 发带围嘴裤袜白袜菠萝毯59</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>白色坑条无袖爬服59</t>
-  </si>
-  <si>
-    <t>ZH20210219A72</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>白色PZ手提箱蕾丝包裙O白飞袖双蝴蝶裙+白无袖爬 发带围嘴裤袜白袜菠萝毯66</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>KC20200425A0102</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZHTM20210218A72</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>天猫-白色PZ手提箱蕾丝包裙O白飞袖双蝴蝶裙+白无袖爬 发带围嘴裤袜白袜菠萝毯66</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>白色坑条无袖爬服66</t>
-  </si>
-  <si>
-    <t>ZH20210219A73</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>白色PZ手提箱蕾丝包裙O白飞袖双蝴蝶裙+白无袖爬 发带围嘴裤袜白袜菠萝毯73</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>KC20210509A0202</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>KC20200425A0103</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZHTM20210218A73</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>天猫-白色PZ手提箱蕾丝包裙O白飞袖双蝴蝶裙+白无袖爬 发带围嘴裤袜白袜菠萝毯73</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>白色坑条无袖爬服73</t>
-  </si>
-  <si>
-    <t>ZH20210219A74</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>白色PZ手提箱蕾丝包裙O白飞袖双蝴蝶裙+白无袖爬 发带围嘴裤袜白袜菠萝毯80</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>KC20200425A0104</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZHTM20210218A74</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>天猫-白色PZ手提箱蕾丝包裙O白飞袖双蝴蝶裙+白无袖爬 发带围嘴裤袜白袜菠萝毯80</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>白色坑条无袖爬服80</t>
-  </si>
-  <si>
-    <t>KC20201217A01</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ZH20210219A75</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>白色PZ手提箱蕾丝包裙O白飞袖双蝴蝶裙+白无袖爬 发带围嘴裤袜白袜菠萝毯90</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ZH20210219A76</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>白色PZ手提箱蕾丝包裙P白飞袖双蝴蝶裙+短袖粉蕾丝裙 发带围嘴裤袜粉袜菠萝毯59</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>KC20210408A0201</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>白色PARKZOO手提箱</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZHTM20210218A75</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>天猫-白色PZ手提箱蕾丝包裙O白飞袖双蝴蝶裙+白无袖爬 发带围嘴裤袜白袜菠萝毯90</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZHTM20210218A76</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>天猫-白色PZ手提箱蕾丝包裙P白飞袖双蝴蝶裙+短袖粉蕾丝裙 发带围嘴裤袜粉袜菠萝毯59</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>粉色蕾丝短袖爬服8425#59</t>
-  </si>
-  <si>
-    <t>KC20210219A01</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>4003粉袜粉花袜子</t>
-  </si>
-  <si>
-    <t>ZH20210219A77</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>白色PZ手提箱蕾丝包裙P白飞袖双蝴蝶裙+短袖粉蕾丝裙 发带围嘴裤袜粉袜菠萝毯66</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>KC20210408A0202</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZHTM20210218A77</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>天猫-白色PZ手提箱蕾丝包裙P白飞袖双蝴蝶裙+短袖粉蕾丝裙 发带围嘴裤袜粉袜菠萝毯66</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>粉色蕾丝短袖爬服8425#66</t>
-  </si>
-  <si>
-    <t>ZH20210219A78</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>白色PZ手提箱蕾丝包裙P白飞袖双蝴蝶裙+短袖粉蕾丝裙 发带围嘴裤袜粉袜菠萝毯73</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>KC20210408A0203</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZHTM20210218A78</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>天猫-白色PZ手提箱蕾丝包裙P白飞袖双蝴蝶裙+短袖粉蕾丝裙 发带围嘴裤袜粉袜菠萝毯73</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>粉色蕾丝短袖爬服8425#73</t>
-  </si>
-  <si>
-    <t>KC20200729D01</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ZH20210219A79</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>白色PZ手提箱蕾丝包裙P白飞袖双蝴蝶裙+短袖粉蕾丝裙 发带围嘴裤袜粉袜菠萝毯80</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>KC20210408A0204</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZHTM20210218A79</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>天猫-白色PZ手提箱蕾丝包裙P白飞袖双蝴蝶裙+短袖粉蕾丝裙 发带围嘴裤袜粉袜菠萝毯80</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>粉色蕾丝短袖爬服8425#80</t>
-  </si>
-  <si>
-    <t>ZH20210219A80</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>白色PZ手提箱蕾丝包裙P白飞袖双蝴蝶裙+短袖粉蕾丝裙 发带围嘴裤袜粉袜菠萝毯90</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZHTM20210218A80</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>天猫-白色PZ手提箱蕾丝包裙P白飞袖双蝴蝶裙+短袖粉蕾丝裙 发带围嘴裤袜粉袜菠萝毯90</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -829,29 +841,29 @@
     </row>
     <row r="2" spans="1:10" ht="14.25">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="F2" s="2">
         <v>488</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="J2" s="2">
         <v>1</v>
@@ -866,10 +878,10 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="J3" s="2">
         <v>1</v>
@@ -884,10 +896,10 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="J4" s="2">
         <v>1</v>
@@ -902,10 +914,10 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="J5" s="2">
         <v>1</v>
@@ -920,10 +932,10 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="J6" s="2">
         <v>1</v>
@@ -938,10 +950,10 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="J7" s="2">
         <v>1</v>
@@ -949,10 +961,10 @@
     </row>
     <row r="8" spans="1:10">
       <c r="H8" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="I8" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -960,10 +972,10 @@
     </row>
     <row r="9" spans="1:10">
       <c r="H9" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="I9" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -971,28 +983,28 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="F10">
         <v>488</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I10" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -1000,10 +1012,10 @@
     </row>
     <row r="11" spans="1:10">
       <c r="H11" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="I11" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -1011,10 +1023,10 @@
     </row>
     <row r="12" spans="1:10">
       <c r="H12" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I12" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -1022,10 +1034,10 @@
     </row>
     <row r="13" spans="1:10">
       <c r="H13" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I13" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -1033,10 +1045,10 @@
     </row>
     <row r="14" spans="1:10">
       <c r="H14" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="I14" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -1044,10 +1056,10 @@
     </row>
     <row r="15" spans="1:10">
       <c r="H15" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="I15" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="J15">
         <v>1</v>
@@ -1055,10 +1067,10 @@
     </row>
     <row r="16" spans="1:10">
       <c r="H16" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="I16" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -1066,10 +1078,10 @@
     </row>
     <row r="17" spans="1:10">
       <c r="H17" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="I17" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="J17">
         <v>1</v>
@@ -1077,28 +1089,28 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="F18">
         <v>488</v>
       </c>
       <c r="H18" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="I18" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -1106,10 +1118,10 @@
     </row>
     <row r="19" spans="1:10">
       <c r="H19" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="I19" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -1117,10 +1129,10 @@
     </row>
     <row r="20" spans="1:10">
       <c r="H20" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="I20" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="J20">
         <v>1</v>
@@ -1128,10 +1140,10 @@
     </row>
     <row r="21" spans="1:10">
       <c r="H21" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I21" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="J21">
         <v>1</v>
@@ -1139,10 +1151,10 @@
     </row>
     <row r="22" spans="1:10">
       <c r="H22" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="I22" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="J22">
         <v>1</v>
@@ -1150,10 +1162,10 @@
     </row>
     <row r="23" spans="1:10">
       <c r="H23" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="I23" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -1161,10 +1173,10 @@
     </row>
     <row r="24" spans="1:10">
       <c r="H24" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="I24" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="J24">
         <v>1</v>
@@ -1172,10 +1184,10 @@
     </row>
     <row r="25" spans="1:10">
       <c r="H25" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="I25" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="J25">
         <v>1</v>
@@ -1183,28 +1195,28 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="D26" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="F26">
         <v>488</v>
       </c>
       <c r="H26" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="I26" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="J26">
         <v>1</v>
@@ -1212,10 +1224,10 @@
     </row>
     <row r="27" spans="1:10">
       <c r="H27" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="I27" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="J27">
         <v>1</v>
@@ -1223,10 +1235,10 @@
     </row>
     <row r="28" spans="1:10">
       <c r="H28" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="I28" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="J28">
         <v>1</v>
@@ -1234,10 +1246,10 @@
     </row>
     <row r="29" spans="1:10">
       <c r="H29" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I29" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="J29">
         <v>1</v>
@@ -1245,10 +1257,10 @@
     </row>
     <row r="30" spans="1:10">
       <c r="H30" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="I30" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="J30">
         <v>1</v>
@@ -1256,10 +1268,10 @@
     </row>
     <row r="31" spans="1:10">
       <c r="H31" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="I31" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="J31">
         <v>1</v>
@@ -1267,10 +1279,10 @@
     </row>
     <row r="32" spans="1:10">
       <c r="H32" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="I32" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="J32">
         <v>1</v>
@@ -1278,10 +1290,10 @@
     </row>
     <row r="33" spans="1:10">
       <c r="H33" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="I33" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="J33">
         <v>1</v>
@@ -1289,28 +1301,28 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C34" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="D34" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E34" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="F34">
         <v>488</v>
       </c>
       <c r="H34" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="I34" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="J34">
         <v>1</v>
@@ -1318,10 +1330,10 @@
     </row>
     <row r="35" spans="1:10">
       <c r="H35" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="I35" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="J35">
         <v>1</v>
@@ -1329,10 +1341,10 @@
     </row>
     <row r="36" spans="1:10">
       <c r="H36" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="I36" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="J36">
         <v>1</v>
@@ -1340,10 +1352,10 @@
     </row>
     <row r="37" spans="1:10">
       <c r="H37" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I37" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="J37">
         <v>1</v>
@@ -1351,10 +1363,10 @@
     </row>
     <row r="38" spans="1:10">
       <c r="H38" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="I38" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="J38">
         <v>1</v>
@@ -1362,10 +1374,10 @@
     </row>
     <row r="39" spans="1:10">
       <c r="H39" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="I39" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="J39">
         <v>1</v>
@@ -1373,10 +1385,10 @@
     </row>
     <row r="40" spans="1:10">
       <c r="H40" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="I40" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="J40">
         <v>1</v>
@@ -1384,10 +1396,10 @@
     </row>
     <row r="41" spans="1:10">
       <c r="H41" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="I41" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="J41">
         <v>1</v>
@@ -1395,28 +1407,28 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B42" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="C42" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="D42" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E42" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="F42">
         <v>488</v>
       </c>
       <c r="H42" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I42" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="J42">
         <v>1</v>
@@ -1424,10 +1436,10 @@
     </row>
     <row r="43" spans="1:10">
       <c r="H43" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="I43" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="J43">
         <v>1</v>
@@ -1435,10 +1447,10 @@
     </row>
     <row r="44" spans="1:10">
       <c r="H44" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I44" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="J44">
         <v>1</v>
@@ -1446,10 +1458,10 @@
     </row>
     <row r="45" spans="1:10">
       <c r="H45" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I45" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="J45">
         <v>1</v>
@@ -1457,10 +1469,10 @@
     </row>
     <row r="46" spans="1:10">
       <c r="H46" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="I46" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="J46">
         <v>1</v>
@@ -1468,10 +1480,10 @@
     </row>
     <row r="47" spans="1:10">
       <c r="H47" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="I47" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="J47">
         <v>1</v>
@@ -1479,10 +1491,10 @@
     </row>
     <row r="48" spans="1:10">
       <c r="H48" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="I48" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="J48">
         <v>1</v>
@@ -1490,10 +1502,10 @@
     </row>
     <row r="49" spans="1:10">
       <c r="H49" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="I49" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="J49">
         <v>1</v>
@@ -1501,28 +1513,28 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B50" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C50" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D50" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E50" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="F50">
         <v>488</v>
       </c>
       <c r="H50" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I50" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="J50">
         <v>1</v>
@@ -1530,10 +1542,10 @@
     </row>
     <row r="51" spans="1:10">
       <c r="H51" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="I51" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="J51">
         <v>1</v>
@@ -1541,10 +1553,10 @@
     </row>
     <row r="52" spans="1:10">
       <c r="H52" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I52" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="J52">
         <v>1</v>
@@ -1552,10 +1564,10 @@
     </row>
     <row r="53" spans="1:10">
       <c r="H53" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I53" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="J53">
         <v>1</v>
@@ -1563,10 +1575,10 @@
     </row>
     <row r="54" spans="1:10">
       <c r="H54" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="I54" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="J54">
         <v>1</v>
@@ -1574,10 +1586,10 @@
     </row>
     <row r="55" spans="1:10">
       <c r="H55" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="I55" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="J55">
         <v>1</v>
@@ -1585,10 +1597,10 @@
     </row>
     <row r="56" spans="1:10">
       <c r="H56" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="I56" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="J56">
         <v>1</v>
@@ -1596,10 +1608,10 @@
     </row>
     <row r="57" spans="1:10">
       <c r="H57" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="I57" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="J57">
         <v>1</v>
@@ -1607,28 +1619,28 @@
     </row>
     <row r="58" spans="1:10">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B58" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C58" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D58" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E58" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="F58">
         <v>488</v>
       </c>
       <c r="H58" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="I58" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J58">
         <v>1</v>
@@ -1636,10 +1648,10 @@
     </row>
     <row r="59" spans="1:10">
       <c r="H59" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="I59" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="J59">
         <v>1</v>
@@ -1647,10 +1659,10 @@
     </row>
     <row r="60" spans="1:10">
       <c r="H60" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="I60" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="J60">
         <v>1</v>
@@ -1658,10 +1670,10 @@
     </row>
     <row r="61" spans="1:10">
       <c r="H61" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I61" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="J61">
         <v>1</v>
@@ -1669,10 +1681,10 @@
     </row>
     <row r="62" spans="1:10">
       <c r="H62" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="I62" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="J62">
         <v>1</v>
@@ -1680,10 +1692,10 @@
     </row>
     <row r="63" spans="1:10">
       <c r="H63" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="I63" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="J63">
         <v>1</v>
@@ -1691,10 +1703,10 @@
     </row>
     <row r="64" spans="1:10">
       <c r="H64" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="I64" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="J64">
         <v>1</v>
@@ -1702,10 +1714,10 @@
     </row>
     <row r="65" spans="1:10">
       <c r="H65" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="I65" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="J65">
         <v>1</v>
@@ -1713,28 +1725,28 @@
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B66" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C66" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D66" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E66" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="F66">
         <v>488</v>
       </c>
       <c r="H66" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="I66" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="J66">
         <v>1</v>
@@ -1742,10 +1754,10 @@
     </row>
     <row r="67" spans="1:10">
       <c r="H67" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="I67" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J67">
         <v>1</v>
@@ -1753,10 +1765,10 @@
     </row>
     <row r="68" spans="1:10">
       <c r="H68" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="I68" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="J68">
         <v>1</v>
@@ -1764,10 +1776,10 @@
     </row>
     <row r="69" spans="1:10">
       <c r="H69" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I69" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="J69">
         <v>1</v>
@@ -1775,10 +1787,10 @@
     </row>
     <row r="70" spans="1:10">
       <c r="H70" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="I70" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="J70">
         <v>1</v>
@@ -1786,10 +1798,10 @@
     </row>
     <row r="71" spans="1:10">
       <c r="H71" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="I71" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="J71">
         <v>1</v>
@@ -1797,10 +1809,10 @@
     </row>
     <row r="72" spans="1:10">
       <c r="H72" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="I72" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="J72">
         <v>1</v>
@@ -1808,10 +1820,10 @@
     </row>
     <row r="73" spans="1:10">
       <c r="H73" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="I73" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="J73">
         <v>1</v>
@@ -1819,28 +1831,28 @@
     </row>
     <row r="74" spans="1:10">
       <c r="A74" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B74" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C74" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D74" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E74" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="F74">
         <v>488</v>
       </c>
       <c r="H74" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="I74" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="J74">
         <v>1</v>
@@ -1848,10 +1860,10 @@
     </row>
     <row r="75" spans="1:10">
       <c r="H75" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="I75" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J75">
         <v>1</v>
@@ -1859,10 +1871,10 @@
     </row>
     <row r="76" spans="1:10">
       <c r="H76" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="I76" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="J76">
         <v>1</v>
@@ -1870,10 +1882,10 @@
     </row>
     <row r="77" spans="1:10">
       <c r="H77" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I77" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="J77">
         <v>1</v>
@@ -1881,10 +1893,10 @@
     </row>
     <row r="78" spans="1:10">
       <c r="H78" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="I78" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="J78">
         <v>1</v>
@@ -1892,10 +1904,10 @@
     </row>
     <row r="79" spans="1:10">
       <c r="H79" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="I79" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="J79">
         <v>1</v>
@@ -1903,10 +1915,10 @@
     </row>
     <row r="80" spans="1:10">
       <c r="H80" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="I80" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="J80">
         <v>1</v>
@@ -1914,10 +1926,10 @@
     </row>
     <row r="81" spans="1:10">
       <c r="H81" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="I81" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="J81">
         <v>1</v>
@@ -1925,28 +1937,28 @@
     </row>
     <row r="82" spans="1:10">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C82" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D82" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E82" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="F82">
         <v>488</v>
       </c>
       <c r="H82" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I82" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="J82">
         <v>1</v>
@@ -1954,10 +1966,10 @@
     </row>
     <row r="83" spans="1:10">
       <c r="H83" t="s">
-        <v>82</v>
+        <v>30</v>
       </c>
       <c r="I83" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J83">
         <v>1</v>
@@ -1965,10 +1977,10 @@
     </row>
     <row r="84" spans="1:10">
       <c r="H84" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I84" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="J84">
         <v>1</v>
@@ -1976,10 +1988,10 @@
     </row>
     <row r="85" spans="1:10">
       <c r="H85" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I85" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="J85">
         <v>1</v>
@@ -1987,10 +1999,10 @@
     </row>
     <row r="86" spans="1:10">
       <c r="H86" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="I86" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="J86">
         <v>1</v>
@@ -1998,10 +2010,10 @@
     </row>
     <row r="87" spans="1:10">
       <c r="H87" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="I87" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="J87">
         <v>1</v>
@@ -2009,10 +2021,10 @@
     </row>
     <row r="88" spans="1:10">
       <c r="H88" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="I88" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="J88">
         <v>1</v>
@@ -2020,10 +2032,10 @@
     </row>
     <row r="89" spans="1:10">
       <c r="H89" t="s">
-        <v>84</v>
+        <v>31</v>
       </c>
       <c r="I89" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J89">
         <v>1</v>
@@ -2031,28 +2043,28 @@
     </row>
     <row r="90" spans="1:10">
       <c r="A90" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B90" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C90" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D90" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E90" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="F90">
         <v>488</v>
       </c>
       <c r="H90" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I90" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="J90">
         <v>1</v>
@@ -2060,7 +2072,7 @@
     </row>
     <row r="91" spans="1:10">
       <c r="H91" t="s">
-        <v>88</v>
+        <v>32</v>
       </c>
       <c r="I91" t="s">
         <v>89</v>
@@ -2071,10 +2083,10 @@
     </row>
     <row r="92" spans="1:10">
       <c r="H92" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I92" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="J92">
         <v>1</v>
@@ -2082,10 +2094,10 @@
     </row>
     <row r="93" spans="1:10">
       <c r="H93" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I93" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="J93">
         <v>1</v>
@@ -2093,10 +2105,10 @@
     </row>
     <row r="94" spans="1:10">
       <c r="H94" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="I94" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="J94">
         <v>1</v>
@@ -2104,10 +2116,10 @@
     </row>
     <row r="95" spans="1:10">
       <c r="H95" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="I95" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="J95">
         <v>1</v>
@@ -2115,10 +2127,10 @@
     </row>
     <row r="96" spans="1:10">
       <c r="H96" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="I96" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="J96">
         <v>1</v>
@@ -2126,10 +2138,10 @@
     </row>
     <row r="97" spans="1:10">
       <c r="H97" t="s">
-        <v>84</v>
+        <v>31</v>
       </c>
       <c r="I97" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J97">
         <v>1</v>
@@ -2146,19 +2158,19 @@
         <v>91</v>
       </c>
       <c r="D98" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E98" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="F98">
         <v>488</v>
       </c>
       <c r="H98" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="I98" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J98">
         <v>1</v>
@@ -2166,10 +2178,10 @@
     </row>
     <row r="99" spans="1:10">
       <c r="H99" t="s">
+        <v>33</v>
+      </c>
+      <c r="I99" t="s">
         <v>92</v>
-      </c>
-      <c r="I99" t="s">
-        <v>93</v>
       </c>
       <c r="J99">
         <v>1</v>
@@ -2177,10 +2189,10 @@
     </row>
     <row r="100" spans="1:10">
       <c r="H100" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="I100" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="J100">
         <v>1</v>
@@ -2188,10 +2200,10 @@
     </row>
     <row r="101" spans="1:10">
       <c r="H101" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I101" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="J101">
         <v>1</v>
@@ -2199,10 +2211,10 @@
     </row>
     <row r="102" spans="1:10">
       <c r="H102" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="I102" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="J102">
         <v>1</v>
@@ -2210,10 +2222,10 @@
     </row>
     <row r="103" spans="1:10">
       <c r="H103" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="I103" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="J103">
         <v>1</v>
@@ -2221,10 +2233,10 @@
     </row>
     <row r="104" spans="1:10">
       <c r="H104" t="s">
-        <v>94</v>
+        <v>17</v>
       </c>
       <c r="I104" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="J104">
         <v>1</v>
@@ -2232,10 +2244,10 @@
     </row>
     <row r="105" spans="1:10">
       <c r="H105" t="s">
-        <v>84</v>
+        <v>31</v>
       </c>
       <c r="I105" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J105">
         <v>1</v>
@@ -2243,28 +2255,28 @@
     </row>
     <row r="106" spans="1:10">
       <c r="A106" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B106" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C106" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D106" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E106" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="F106">
         <v>488</v>
       </c>
       <c r="H106" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="I106" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="J106">
         <v>1</v>
@@ -2272,10 +2284,10 @@
     </row>
     <row r="107" spans="1:10">
       <c r="H107" t="s">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="I107" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J107">
         <v>1</v>
@@ -2283,10 +2295,10 @@
     </row>
     <row r="108" spans="1:10">
       <c r="H108" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="I108" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="J108">
         <v>1</v>
@@ -2294,10 +2306,10 @@
     </row>
     <row r="109" spans="1:10">
       <c r="H109" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I109" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="J109">
         <v>1</v>
@@ -2305,10 +2317,10 @@
     </row>
     <row r="110" spans="1:10">
       <c r="H110" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="I110" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="J110">
         <v>1</v>
@@ -2316,10 +2328,10 @@
     </row>
     <row r="111" spans="1:10">
       <c r="H111" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="I111" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="J111">
         <v>1</v>
@@ -2327,10 +2339,10 @@
     </row>
     <row r="112" spans="1:10">
       <c r="H112" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="I112" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="J112">
         <v>1</v>
@@ -2338,10 +2350,10 @@
     </row>
     <row r="113" spans="1:10">
       <c r="H113" t="s">
-        <v>84</v>
+        <v>31</v>
       </c>
       <c r="I113" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J113">
         <v>1</v>
@@ -2349,28 +2361,28 @@
     </row>
     <row r="114" spans="1:10">
       <c r="A114" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B114" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C114" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D114" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E114" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="F114">
         <v>488</v>
       </c>
       <c r="H114" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="I114" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="J114">
         <v>1</v>
@@ -2378,10 +2390,10 @@
     </row>
     <row r="115" spans="1:10">
       <c r="H115" t="s">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="I115" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J115">
         <v>1</v>
@@ -2389,10 +2401,10 @@
     </row>
     <row r="116" spans="1:10">
       <c r="H116" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="I116" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="J116">
         <v>1</v>
@@ -2400,10 +2412,10 @@
     </row>
     <row r="117" spans="1:10">
       <c r="H117" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I117" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="J117">
         <v>1</v>
@@ -2411,10 +2423,10 @@
     </row>
     <row r="118" spans="1:10">
       <c r="H118" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="I118" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="J118">
         <v>1</v>
@@ -2422,10 +2434,10 @@
     </row>
     <row r="119" spans="1:10">
       <c r="H119" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="I119" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="J119">
         <v>1</v>
@@ -2433,10 +2445,10 @@
     </row>
     <row r="120" spans="1:10">
       <c r="H120" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="I120" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="J120">
         <v>1</v>
@@ -2444,10 +2456,10 @@
     </row>
     <row r="121" spans="1:10">
       <c r="H121" t="s">
-        <v>84</v>
+        <v>31</v>
       </c>
       <c r="I121" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J121">
         <v>1</v>

</xml_diff>